<commit_message>
Uploaded 19-May-2020 07:21:54 {/src/main/resources/com/techm/bm/om/brms/InstallBaseIDGeneration.xlsx}
</commit_message>
<xml_diff>
--- a/src/main/resources/com/techm/bm/om/brms/InstallBaseIDGeneration.xlsx
+++ b/src/main/resources/com/techm/bm/om/brms/InstallBaseIDGeneration.xlsx
@@ -83,7 +83,7 @@
     <t>com.techm.bm.om.brms.InstallBaseIDGeneration</t>
   </si>
   <si>
-    <t>HST</t>
+    <t>IMEA Number</t>
   </si>
 </sst>
 </file>
@@ -668,10 +668,10 @@
       <c r="C13" s="13" t="s">
         <v>14</v>
       </c>
-      <c r="D13" s="13"/>
-      <c r="E13" s="13" t="s">
+      <c r="D13" s="13" t="s">
         <v>20</v>
       </c>
+      <c r="E13" s="13"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>